<commit_message>
Update SYP Projekt Money Managment.xlsx
</commit_message>
<xml_diff>
--- a/hardware/SYP Projekt Money Managment.xlsx
+++ b/hardware/SYP Projekt Money Managment.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/moritz/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/moritz/Documents/GitHub/HulaSwirl/hardware/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{28E0C3D1-C1CA-1A43-948F-AE96BABB2EEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3BBD73C-ED79-FE4E-A3D0-101777840AE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="24320" xr2:uid="{5C2BC352-EA72-3047-A569-738E49AE4B2F}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
   <si>
     <t>SYP Project</t>
   </si>
@@ -124,6 +123,12 @@
   </si>
   <si>
     <t>wire usb-a to usb-c</t>
+  </si>
+  <si>
+    <t>https://www.amazon.de/-/en/LAVMHAB-Silicone-Flexible-Pumping-Transfer/dp/B0D9NRLR1K?crid=2O9NW9O1OLT95&amp;dib=eyJ2IjoiMSJ9.FCrh94MEEO0jp4-k4fQGxYMMit5zN8Ddzby2BDyEk_UCjtk5-yg4-0wtAVgOpdvtJPhVu5nHl7yQQ_OHwYc5ZDKkRoLd3MJQr3SzEbZ9XvGr4whdEfGauaxCsqcwoGINfLkiOMZ8UWXYtKcGZ75nICn1K4kxyaDTrK6Kbp4VFcNp2QmsZN7TEfri5icLJBDTrbwDlcSHkvuQJmqD_u3aviGNadizMwUQCy1ILMNom7oc3HvyXUFJgnUfMLOP75BCp-aI-RKrtz4vaYyVyocRhJOfuYPtpJOi2f2kxZu0wzo.3ozZ4Wradsj81AlhWYepdDAu5nTMiNkJFeO6_YZtgps&amp;dib_tag=se&amp;keywords=silikonschlauch%2B5mm&amp;nsdOptOutParam=true&amp;qid=1732518622&amp;sprefix=5mm%2Bsilic%2Caps%2C109&amp;sr=8-17&amp;th=1</t>
+  </si>
+  <si>
+    <t>silicon cable</t>
   </si>
 </sst>
 </file>
@@ -538,10 +543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F860369-660E-9242-9C25-0ADA69D6C52D}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="293" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -809,24 +814,53 @@
         <f>C15/3</f>
         <v>1.7133333333333332</v>
       </c>
+      <c r="G15" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="A16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="4">
+        <v>10.07</v>
+      </c>
+      <c r="D16" s="4">
+        <f>C16/3</f>
+        <v>3.3566666666666669</v>
+      </c>
+      <c r="E16" s="4">
+        <f>C16/3</f>
+        <v>3.3566666666666669</v>
+      </c>
+      <c r="F16" s="4">
+        <f>C16/3</f>
+        <v>3.3566666666666669</v>
+      </c>
+      <c r="G16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="4">
-        <f>SUM(C7:C15)</f>
-        <v>110.92</v>
-      </c>
-      <c r="D16" s="4">
+      <c r="C17" s="4">
+        <f>SUM(C7:C16)</f>
+        <v>120.99000000000001</v>
+      </c>
+      <c r="D17" s="4">
         <f>SUM(D7:D14) -6</f>
         <v>29.260000000000005</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E17" s="4">
         <f>SUM(E7:E14) - 6</f>
         <v>29.260000000000005</v>
       </c>
-      <c r="F16" s="4">
+      <c r="F17" s="4">
         <f>SUM(F7:F14)</f>
         <v>35.260000000000005</v>
       </c>
@@ -837,6 +871,7 @@
     <hyperlink ref="B10" r:id="rId2" display="https://www.amazon.de/-/en/Flintronic-Connectors-Actuation-Electrical-Connection/dp/B0BCNTVV4S?crid=3A2VIYI1QSS7Z&amp;dib=eyJ2IjoiMSJ9.5EQ8zrESx451OzCIIRy8TynGNCOOU_tx5kUwW57W39fluXdRPrPP0f9UMO9k3e4VdSOlzl9TcVhBx1AwtOP5ZevuMXOBOZL_gD4RFGnX0ccMBFToECeX1zHkysg5lHoOx7xzxiVtn4nUQPEUeIIFyLax-Fnbb4eekQKGEzmLSbANhMBjuSTHugEnY4Ff7GfenpIukaHeJaSqtrRdbGDnYjC2QNWXqUBrE6RKQm3vRa_0bgcbWrMAIVA824JsThaz5mpfZWwGrQADgP9lRSYO5laykRqokroZzqjWNLgVca0.X8jhVTC-kOL7SmM2QrBLVj0YrzamKj5jYkA3vn__00U&amp;dib_tag=se&amp;keywords=connect+cable&amp;qid=1730973101&amp;sprefix=connect+cabl%2Caps%2C109&amp;sr=8-9" xr:uid="{C59039E8-733C-2545-9BDD-AAAA6E5B2B54}"/>
     <hyperlink ref="B11" r:id="rId3" display="https://www.amazon.de/-/en/Silicone-Electric-Stranded-Electrical-Applications/dp/B0C7QTH8TC?crid=1KOPOHRL7HRBO&amp;dib=eyJ2IjoiMSJ9.VN-g2lxkL868stgPOid0hK-Z35gETrYV7C5EdQnFRzCZPsqORFx4Z_SH0RIZNgQYu2g9FpvYaxyd_MPuPCVTQdhz6uTaWkiVfefgJlKxr4HNxHihUeOjAN50T7r3Gefnbucow4WWhrTsmZ2TixYfvY0uSpUlG7JzCKswtQBkrttnwUdIazaP57FE8hWmhzsscCl8KabjG1RCoePhFvPVkvQsKLcIAe5IiU7VmTSNhgLq85Q3f06uVFUIjoEhsyG2ioaEdXMOBR0fOzU-giWJTTrlyM35I8cGNH2FFfktH2o.yEOPCQuFURyct9ee-pa2RtkbTOGPW0ecgD_wWKWI_90&amp;dib_tag=se&amp;keywords=18%2BAWG%2Bwire&amp;qid=1730973174&amp;sprefix=18%2Bawg%2Bwir%2Caps%2C100&amp;sr=8-18&amp;th=1" xr:uid="{5FB2176A-9876-CA4A-AD56-F464E92C2DF6}"/>
     <hyperlink ref="B12" r:id="rId4" display="https://www.amazon.de/-/en/Adapter-100-240-Transformer-Monitor-Amplifier-Power-supply-12-V-3/dp/B0BP66JZLX?crid=2L6PFKLCEVK81&amp;dib=eyJ2IjoiMSJ9._lkwspqmhU_fj9XvC2uB5Cll1bhHvjucTD1A1D93tQk0JwlyQ4i6_3KLH50N6DVbERmRfGBI-todPqX7FLL5o5m57lb4gFZdm8kdYJ72AwpwxX-6JuOLioxnVWqHmBiIfDy4Fyy2Cytbg1BVEG4vdmPcsibKb6P96-IsLemjw9XJiA0fi4SjBPL8Zhhijl2xy5fPbpkNvHEwu6iooqHzu_G1vLNEElQQjCUVDi00Y8c.mPqtxyoN5vhUvYyrQxUjrDtudTG9thY3_s2Dg8dyO-E&amp;dib_tag=se&amp;keywords=power+supply+3A&amp;qid=1731005289&amp;sprefix=power+supply+3a%2Caps%2C120&amp;sr=8-3" xr:uid="{67CE83EB-22FA-5644-92FE-AAC5FA9F7963}"/>
+    <hyperlink ref="B16" r:id="rId5" display="https://www.amazon.de/-/en/LAVMHAB-Silicone-Flexible-Pumping-Transfer/dp/B0D9NRLR1K?crid=2O9NW9O1OLT95&amp;dib=eyJ2IjoiMSJ9.FCrh94MEEO0jp4-k4fQGxYMMit5zN8Ddzby2BDyEk_UCjtk5-yg4-0wtAVgOpdvtJPhVu5nHl7yQQ_OHwYc5ZDKkRoLd3MJQr3SzEbZ9XvGr4whdEfGauaxCsqcwoGINfLkiOMZ8UWXYtKcGZ75nICn1K4kxyaDTrK6Kbp4VFcNp2QmsZN7TEfri5icLJBDTrbwDlcSHkvuQJmqD_u3aviGNadizMwUQCy1ILMNom7oc3HvyXUFJgnUfMLOP75BCp-aI-RKrtz4vaYyVyocRhJOfuYPtpJOi2f2kxZu0wzo.3ozZ4Wradsj81AlhWYepdDAu5nTMiNkJFeO6_YZtgps&amp;dib_tag=se&amp;keywords=silikonschlauch%2B5mm&amp;nsdOptOutParam=true&amp;qid=1732518622&amp;sprefix=5mm%2Bsilic%2Caps%2C109&amp;sr=8-17&amp;th=1" xr:uid="{7A509784-FB60-D24C-B059-CCF46621FB50}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
electronik bestellt, this closes #9
</commit_message>
<xml_diff>
--- a/hardware/SYP Projekt Money Managment.xlsx
+++ b/hardware/SYP Projekt Money Managment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/moritz/Documents/GitHub/HulaSwirl/hardware/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B30FEC78-6387-8B4D-9FC5-E612E6A91019}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1442AFB6-9C71-7842-AA35-5832690606D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="24320" xr2:uid="{5C2BC352-EA72-3047-A569-738E49AE4B2F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="41">
   <si>
     <t>SYP Project</t>
   </si>
@@ -138,6 +138,27 @@
   </si>
   <si>
     <t>old</t>
+  </si>
+  <si>
+    <t>bestellt</t>
+  </si>
+  <si>
+    <t>Bestellung 1</t>
+  </si>
+  <si>
+    <t>Bestellung 2</t>
+  </si>
+  <si>
+    <t>Prototyp mit 1 Netzteil (NICHT IN VERWENDUNG)</t>
+  </si>
+  <si>
+    <t>Prototyp mit 2 Netzteilen (IN VERWENDUNG)</t>
+  </si>
+  <si>
+    <t>SUM</t>
+  </si>
+  <si>
+    <t>remaining</t>
   </si>
 </sst>
 </file>
@@ -147,7 +168,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_ [$€-2]\ * #,##0.00_ ;_ [$€-2]\ * \-#,##0.00_ ;_ [$€-2]\ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -166,6 +187,13 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -210,13 +238,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -552,10 +581,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F860369-660E-9242-9C25-0ADA69D6C52D}">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="207" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="207" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -569,6 +598,11 @@
         <v>0</v>
       </c>
     </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>33</v>
@@ -884,6 +918,11 @@
         <v>30</v>
       </c>
     </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>38</v>
+      </c>
+    </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>1</v>
@@ -956,7 +995,7 @@
         <v>4.7033333333333331</v>
       </c>
       <c r="G26" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
@@ -992,7 +1031,7 @@
         <v>2.6833333333333336</v>
       </c>
       <c r="G28" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
@@ -1003,22 +1042,22 @@
         <v>18</v>
       </c>
       <c r="C29" s="4">
-        <v>13.1</v>
+        <v>12.44</v>
       </c>
       <c r="D29" s="4">
         <f t="shared" si="3"/>
-        <v>4.3666666666666663</v>
+        <v>4.1466666666666665</v>
       </c>
       <c r="E29" s="4">
         <f t="shared" si="4"/>
-        <v>4.3666666666666663</v>
+        <v>4.1466666666666665</v>
       </c>
       <c r="F29" s="4">
         <f t="shared" si="5"/>
-        <v>4.3666666666666663</v>
+        <v>4.1466666666666665</v>
       </c>
       <c r="G29" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -1044,14 +1083,14 @@
         <v>4.4533333333333331</v>
       </c>
       <c r="G30" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C31" s="4">
@@ -1070,7 +1109,7 @@
         <v>4.3666666666666663</v>
       </c>
       <c r="G31" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
@@ -1097,7 +1136,7 @@
         <v>6.04</v>
       </c>
       <c r="G32" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
@@ -1132,7 +1171,7 @@
         <v>3.3566666666666669</v>
       </c>
       <c r="G34" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
@@ -1141,19 +1180,19 @@
       </c>
       <c r="C35" s="4">
         <f>SUM(C25:C34)</f>
-        <v>107.91</v>
+        <v>107.25</v>
       </c>
       <c r="D35" s="4">
         <f>SUM(D25:D32) -6</f>
-        <v>26.613333333333337</v>
+        <v>26.393333333333331</v>
       </c>
       <c r="E35" s="4">
         <f>SUM(E25:E32) - 6</f>
-        <v>26.613333333333337</v>
+        <v>26.393333333333331</v>
       </c>
       <c r="F35" s="4">
         <f>SUM(F25:F32)</f>
-        <v>32.613333333333337</v>
+        <v>32.393333333333331</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
@@ -1162,12 +1201,44 @@
       </c>
       <c r="C36" s="4">
         <f>130-C35</f>
-        <v>22.090000000000003</v>
+        <v>22.75</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C37" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C40" t="s">
+        <v>35</v>
+      </c>
+      <c r="D40" t="s">
+        <v>36</v>
+      </c>
+      <c r="E40" t="s">
+        <v>39</v>
+      </c>
+      <c r="F40" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C41" s="4">
+        <f>C25</f>
+        <v>18</v>
+      </c>
+      <c r="D41" s="4">
+        <f>C35-18</f>
+        <v>89.25</v>
+      </c>
+      <c r="E41" s="4">
+        <f>SUM(C41:D41)</f>
+        <v>107.25</v>
+      </c>
+      <c r="F41" s="4">
+        <f>130-E41</f>
+        <v>22.75</v>
       </c>
     </row>
   </sheetData>
@@ -1183,6 +1254,7 @@
     <hyperlink ref="B30" r:id="rId9" display="https://www.amazon.de/-/en/Adapter-100-240-Transformer-Monitor-Amplifier-Power-supply-12-V-3/dp/B0BP66JZLX?crid=2L6PFKLCEVK81&amp;dib=eyJ2IjoiMSJ9._lkwspqmhU_fj9XvC2uB5Cll1bhHvjucTD1A1D93tQk0JwlyQ4i6_3KLH50N6DVbERmRfGBI-todPqX7FLL5o5m57lb4gFZdm8kdYJ72AwpwxX-6JuOLioxnVWqHmBiIfDy4Fyy2Cytbg1BVEG4vdmPcsibKb6P96-IsLemjw9XJiA0fi4SjBPL8Zhhijl2xy5fPbpkNvHEwu6iooqHzu_G1vLNEElQQjCUVDi00Y8c.mPqtxyoN5vhUvYyrQxUjrDtudTG9thY3_s2Dg8dyO-E&amp;dib_tag=se&amp;keywords=power+supply+3A&amp;qid=1731005289&amp;sprefix=power+supply+3a%2Caps%2C120&amp;sr=8-3" xr:uid="{75D88FC1-C021-B242-AEE2-8C0FD7B46613}"/>
     <hyperlink ref="B34" r:id="rId10" display="https://www.amazon.de/-/en/LAVMHAB-Silicone-Flexible-Pumping-Transfer/dp/B0D9NRLR1K?crid=2O9NW9O1OLT95&amp;dib=eyJ2IjoiMSJ9.FCrh94MEEO0jp4-k4fQGxYMMit5zN8Ddzby2BDyEk_UCjtk5-yg4-0wtAVgOpdvtJPhVu5nHl7yQQ_OHwYc5ZDKkRoLd3MJQr3SzEbZ9XvGr4whdEfGauaxCsqcwoGINfLkiOMZ8UWXYtKcGZ75nICn1K4kxyaDTrK6Kbp4VFcNp2QmsZN7TEfri5icLJBDTrbwDlcSHkvuQJmqD_u3aviGNadizMwUQCy1ILMNom7oc3HvyXUFJgnUfMLOP75BCp-aI-RKrtz4vaYyVyocRhJOfuYPtpJOi2f2kxZu0wzo.3ozZ4Wradsj81AlhWYepdDAu5nTMiNkJFeO6_YZtgps&amp;dib_tag=se&amp;keywords=silikonschlauch%2B5mm&amp;nsdOptOutParam=true&amp;qid=1732518622&amp;sprefix=5mm%2Bsilic%2Caps%2C109&amp;sr=8-17&amp;th=1" xr:uid="{D2CA59AA-CA1B-7D43-B098-F516CCF40A92}"/>
     <hyperlink ref="B7" r:id="rId11" xr:uid="{F91F929A-3AB0-2C46-8AA0-7385C8A2708B}"/>
+    <hyperlink ref="B31" r:id="rId12" display="https://www.amazon.de/-/en/HUAREW-Breadboard-Dupont-Points-Arduino/dp/B0B5TCKTQH?crid=2H1V44Q263MD5&amp;dib=eyJ2IjoiMSJ9.aRQeJMI5vdGBirt5tCbbkvFrQGta46bFt4TW95QpKEI_qHNschVOZrDLg2LZDJJZQAXxyh-2uU9z9h8oMATldodApJRJ3Aw0v33jJoYkZPAIOUjT6Rn-n3cJCxTrRwhqyIvsNW9NoxCx8P_a7BCcYzp2_8deppQsQIBABuIQxDvttl7ca73gW1j-YaZYmrjlH1v6Ai5UeNeYgtCnwP9a1o27a4E_BofieoY3sTTA0scZIUI-Q_9jp4Pp4yylzZ1g0V7kDiI2c-HRnldF07111cC90ts6DsUeTzG2M4DqR58.GKKUBGBXDt9iH5LYVhwsJuKDZRnn8kGujHwg4HpLXqc&amp;dib_tag=se&amp;keywords=steckplatine&amp;qid=1730977442&amp;sprefix=steckplatine%2Caps%2C145&amp;sr=8-15" xr:uid="{1FBA583B-B7E5-6445-A245-065661D88F99}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>